<commit_message>
update 21 may 2024 11.49
</commit_message>
<xml_diff>
--- a/dataset/potential-rain.xlsx
+++ b/dataset/potential-rain.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Documents/kriti/kuliah/Skripsi/semhas/dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Documents/kriti/Developments/python/prediction-speed-courir/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5807498C-C058-244B-A42E-F69FE8C0BD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C9B01A-419C-AC4F-A051-B750AC6FB645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18260" yWindow="-18920" windowWidth="10000" windowHeight="16080" xr2:uid="{B51C871F-C235-934F-9723-8FB515E3EE6A}"/>
+    <workbookView xWindow="-620" yWindow="500" windowWidth="10000" windowHeight="16080" xr2:uid="{B51C871F-C235-934F-9723-8FB515E3EE6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -398,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7640E8E8-793C-514A-A1D2-B122A158555C}">
   <dimension ref="A1:C185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="C158" sqref="C158"/>
+    <sheetView tabSelected="1" zoomScale="182" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -422,31 +422,67 @@
       <c r="A2" s="1">
         <v>45108</v>
       </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>45109</v>
       </c>
+      <c r="B3">
+        <v>40</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>45110</v>
       </c>
+      <c r="B4">
+        <v>35</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>45111</v>
       </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>45112</v>
       </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>45113</v>
       </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -474,76 +510,166 @@
       <c r="A10" s="1">
         <v>45116</v>
       </c>
+      <c r="B10">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>45117</v>
       </c>
+      <c r="B11">
+        <v>40</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>45118</v>
       </c>
+      <c r="B12">
+        <v>40</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>45119</v>
       </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>45120</v>
       </c>
+      <c r="B14">
+        <v>40</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>45121</v>
       </c>
+      <c r="B15">
+        <v>35</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>45122</v>
       </c>
+      <c r="B16">
+        <v>50</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>45123</v>
       </c>
+      <c r="B17">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>45124</v>
       </c>
+      <c r="B18">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>45125</v>
       </c>
+      <c r="B19">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>45126</v>
       </c>
+      <c r="B20">
+        <v>40</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>45127</v>
       </c>
+      <c r="B21">
+        <v>40</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>45128</v>
       </c>
+      <c r="B22">
+        <v>30</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>45129</v>
       </c>
+      <c r="B23">
+        <v>50</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>45130</v>
       </c>
+      <c r="B24">
+        <v>40</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -560,6 +686,12 @@
       <c r="A26" s="1">
         <v>45132</v>
       </c>
+      <c r="B26">
+        <v>50</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -576,156 +708,342 @@
       <c r="A28" s="1">
         <v>45134</v>
       </c>
+      <c r="B28">
+        <v>50</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>45135</v>
       </c>
+      <c r="B29">
+        <v>50</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>45136</v>
       </c>
+      <c r="B30">
+        <v>40</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>45137</v>
       </c>
+      <c r="B31">
+        <v>50</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>45138</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>40</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>45139</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>40</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>45140</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>45141</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>40</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>45142</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>50</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>45143</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>40</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>45144</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <v>40</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>45145</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <v>35</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>45146</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>40</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>45147</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>45148</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <v>50</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>45149</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B43">
+        <v>50</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>45150</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B44">
+        <v>40</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>45151</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B45">
+        <v>35</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45152</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B46">
+        <v>40</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45153</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B47">
+        <v>35</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>45154</v>
+      </c>
+      <c r="B48">
+        <v>40</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>45155</v>
       </c>
+      <c r="B49">
+        <v>40</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>45156</v>
       </c>
+      <c r="B50">
+        <v>40</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>45157</v>
       </c>
+      <c r="B51">
+        <v>40</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>45158</v>
       </c>
+      <c r="B52">
+        <v>35</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>45159</v>
       </c>
+      <c r="B53">
+        <v>50</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>45160</v>
       </c>
+      <c r="B54">
+        <v>35</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>45161</v>
       </c>
+      <c r="B55">
+        <v>35</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>45162</v>
       </c>
+      <c r="B56">
+        <v>40</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>45163</v>
       </c>
+      <c r="B57">
+        <v>50</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>45164</v>
       </c>
+      <c r="B58">
+        <v>40</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
@@ -742,36 +1060,78 @@
       <c r="A60" s="1">
         <v>45166</v>
       </c>
+      <c r="B60">
+        <v>40</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>45167</v>
       </c>
+      <c r="B61">
+        <v>50</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>45168</v>
       </c>
+      <c r="B62">
+        <v>40</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>45169</v>
       </c>
+      <c r="B63">
+        <v>40</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>45170</v>
       </c>
+      <c r="B64">
+        <v>35</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>45171</v>
       </c>
+      <c r="B65">
+        <v>40</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>45172</v>
       </c>
+      <c r="B66">
+        <v>35</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
@@ -788,51 +1148,111 @@
       <c r="A68" s="1">
         <v>45174</v>
       </c>
+      <c r="B68">
+        <v>40</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>45175</v>
       </c>
+      <c r="B69">
+        <v>35</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>45176</v>
       </c>
+      <c r="B70">
+        <v>40</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>45177</v>
       </c>
+      <c r="B71">
+        <v>40</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>45178</v>
       </c>
+      <c r="B72">
+        <v>45</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>45179</v>
       </c>
+      <c r="B73">
+        <v>35</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>45180</v>
       </c>
+      <c r="B74">
+        <v>35</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>45181</v>
       </c>
+      <c r="B75">
+        <v>35</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>45182</v>
       </c>
+      <c r="B76">
+        <v>40</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>45183</v>
       </c>
+      <c r="B77">
+        <v>40</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
@@ -849,96 +1269,210 @@
       <c r="A79" s="1">
         <v>45185</v>
       </c>
+      <c r="B79">
+        <v>50</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>45186</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B80">
+        <v>40</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>45187</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B81">
+        <v>50</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>45188</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>50</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>45189</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B83">
+        <v>35</v>
+      </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>45190</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B84">
+        <v>35</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>45191</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B85">
+        <v>40</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>45192</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B86">
+        <v>40</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>45193</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B87">
+        <v>35</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>45194</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B88">
+        <v>50</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>45195</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B89">
+        <v>40</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>45196</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B90">
+        <v>40</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>45197</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B91">
+        <v>40</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>45198</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>50</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>45199</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B93">
+        <v>30</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>45200</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B94">
+        <v>35</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>45201</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B95">
+        <v>35</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>45202</v>
+      </c>
+      <c r="B96">
+        <v>40</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>45203</v>
       </c>
+      <c r="B97">
+        <v>60</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
@@ -955,16 +1489,34 @@
       <c r="A99" s="1">
         <v>45205</v>
       </c>
+      <c r="B99">
+        <v>40</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>45206</v>
       </c>
+      <c r="B100">
+        <v>40</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>45207</v>
       </c>
+      <c r="B101">
+        <v>40</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
@@ -1003,26 +1555,56 @@
       <c r="A105" s="1">
         <v>45211</v>
       </c>
+      <c r="B105">
+        <v>50</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>45212</v>
       </c>
+      <c r="B106">
+        <v>40</v>
+      </c>
+      <c r="C106">
+        <v>1</v>
+      </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>45213</v>
       </c>
+      <c r="B107">
+        <v>40</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>45214</v>
       </c>
+      <c r="B108">
+        <v>40</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>45215</v>
       </c>
+      <c r="B109">
+        <v>40</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
@@ -1039,11 +1621,23 @@
       <c r="A111" s="1">
         <v>45217</v>
       </c>
+      <c r="B111">
+        <v>35</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>45218</v>
       </c>
+      <c r="B112">
+        <v>40</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
@@ -1071,6 +1665,12 @@
       <c r="A115" s="1">
         <v>45221</v>
       </c>
+      <c r="B115">
+        <v>50</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
@@ -1087,6 +1687,12 @@
       <c r="A117" s="1">
         <v>45223</v>
       </c>
+      <c r="B117">
+        <v>50</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
@@ -1103,26 +1709,56 @@
       <c r="A119" s="1">
         <v>45225</v>
       </c>
+      <c r="B119">
+        <v>50</v>
+      </c>
+      <c r="C119">
+        <v>1</v>
+      </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>45226</v>
       </c>
+      <c r="B120">
+        <v>40</v>
+      </c>
+      <c r="C120">
+        <v>1</v>
+      </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>45227</v>
       </c>
+      <c r="B121">
+        <v>35</v>
+      </c>
+      <c r="C121">
+        <v>1</v>
+      </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>45228</v>
       </c>
+      <c r="B122">
+        <v>35</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>45229</v>
       </c>
+      <c r="B123">
+        <v>40</v>
+      </c>
+      <c r="C123">
+        <v>1</v>
+      </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
@@ -1150,6 +1786,12 @@
       <c r="A126" s="1">
         <v>45232</v>
       </c>
+      <c r="B126">
+        <v>60</v>
+      </c>
+      <c r="C126">
+        <v>1</v>
+      </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
@@ -1188,26 +1830,56 @@
       <c r="A130" s="1">
         <v>45236</v>
       </c>
+      <c r="B130">
+        <v>40</v>
+      </c>
+      <c r="C130">
+        <v>1</v>
+      </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>45237</v>
       </c>
+      <c r="B131">
+        <v>50</v>
+      </c>
+      <c r="C131">
+        <v>1</v>
+      </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>45238</v>
       </c>
+      <c r="B132">
+        <v>50</v>
+      </c>
+      <c r="C132">
+        <v>1</v>
+      </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>45239</v>
       </c>
+      <c r="B133">
+        <v>45</v>
+      </c>
+      <c r="C133">
+        <v>1</v>
+      </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>45240</v>
       </c>
+      <c r="B134">
+        <v>50</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
@@ -1235,6 +1907,12 @@
       <c r="A137" s="1">
         <v>45243</v>
       </c>
+      <c r="B137">
+        <v>50</v>
+      </c>
+      <c r="C137">
+        <v>1</v>
+      </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
@@ -1273,6 +1951,12 @@
       <c r="A141" s="1">
         <v>45247</v>
       </c>
+      <c r="B141">
+        <v>50</v>
+      </c>
+      <c r="C141">
+        <v>1</v>
+      </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
@@ -1289,11 +1973,23 @@
       <c r="A143" s="1">
         <v>45249</v>
       </c>
+      <c r="B143">
+        <v>40</v>
+      </c>
+      <c r="C143">
+        <v>1</v>
+      </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>45250</v>
       </c>
+      <c r="B144">
+        <v>50</v>
+      </c>
+      <c r="C144">
+        <v>1</v>
+      </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
@@ -1310,11 +2006,23 @@
       <c r="A146" s="1">
         <v>45252</v>
       </c>
+      <c r="B146">
+        <v>50</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
+      </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>45253</v>
       </c>
+      <c r="B147">
+        <v>50</v>
+      </c>
+      <c r="C147">
+        <v>1</v>
+      </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
@@ -1331,6 +2039,12 @@
       <c r="A149" s="1">
         <v>45255</v>
       </c>
+      <c r="B149">
+        <v>50</v>
+      </c>
+      <c r="C149">
+        <v>1</v>
+      </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
@@ -1347,6 +2061,12 @@
       <c r="A151" s="1">
         <v>45257</v>
       </c>
+      <c r="B151">
+        <v>50</v>
+      </c>
+      <c r="C151">
+        <v>1</v>
+      </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
@@ -1363,6 +2083,12 @@
       <c r="A153" s="1">
         <v>45259</v>
       </c>
+      <c r="B153">
+        <v>40</v>
+      </c>
+      <c r="C153">
+        <v>1</v>
+      </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
@@ -1423,6 +2149,12 @@
       <c r="A159" s="1">
         <v>45265</v>
       </c>
+      <c r="B159">
+        <v>40</v>
+      </c>
+      <c r="C159">
+        <v>1</v>
+      </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
@@ -1439,6 +2171,12 @@
       <c r="A161" s="1">
         <v>45267</v>
       </c>
+      <c r="B161">
+        <v>35</v>
+      </c>
+      <c r="C161">
+        <v>1</v>
+      </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
@@ -1488,61 +2226,133 @@
       <c r="A166" s="1">
         <v>45272</v>
       </c>
+      <c r="B166">
+        <v>40</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
+      </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>45273</v>
       </c>
+      <c r="B167">
+        <v>40</v>
+      </c>
+      <c r="C167">
+        <v>1</v>
+      </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>45274</v>
       </c>
+      <c r="B168">
+        <v>35</v>
+      </c>
+      <c r="C168">
+        <v>1</v>
+      </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>45275</v>
       </c>
+      <c r="B169">
+        <v>40</v>
+      </c>
+      <c r="C169">
+        <v>1</v>
+      </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>45276</v>
       </c>
+      <c r="B170">
+        <v>40</v>
+      </c>
+      <c r="C170">
+        <v>1</v>
+      </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>45277</v>
       </c>
+      <c r="B171">
+        <v>40</v>
+      </c>
+      <c r="C171">
+        <v>1</v>
+      </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>45278</v>
       </c>
+      <c r="B172">
+        <v>40</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>45279</v>
       </c>
+      <c r="B173">
+        <v>35</v>
+      </c>
+      <c r="C173">
+        <v>1</v>
+      </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>45280</v>
       </c>
+      <c r="B174">
+        <v>30</v>
+      </c>
+      <c r="C174">
+        <v>1</v>
+      </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>45281</v>
       </c>
+      <c r="B175">
+        <v>35</v>
+      </c>
+      <c r="C175">
+        <v>1</v>
+      </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>45282</v>
       </c>
+      <c r="B176">
+        <v>50</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>45283</v>
       </c>
+      <c r="B177">
+        <v>40</v>
+      </c>
+      <c r="C177">
+        <v>1</v>
+      </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
@@ -1569,6 +2379,12 @@
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>45286</v>
+      </c>
+      <c r="B180">
+        <v>50</v>
+      </c>
+      <c r="C180">
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>